<commit_message>
Update last end point and rename - seguTiendaSekuraUploadFile
</commit_message>
<xml_diff>
--- a/arq/Tablas_Significado.xlsx
+++ b/arq/Tablas_Significado.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FZGC\AER_PassiDocs_Natural\arq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870840DA-C85C-48A9-8155-FA295511E119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA0F3EC-1F67-48B8-943F-5DE37054B42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{690E9754-8DAB-491D-B572-8F25C1E44882}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{690E9754-8DAB-491D-B572-8F25C1E44882}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tablas" sheetId="1" r:id="rId1"/>
+    <sheet name="segutiendasekurauploadfile" sheetId="2" r:id="rId1"/>
+    <sheet name="Tablas" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="289">
   <si>
     <t>docs_group</t>
   </si>
@@ -1059,6 +1060,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9B2A27B1-2ED2-454F-94FA-485094C1D042}" name="Tabla17" displayName="Tabla17" ref="A2:D8" totalsRowShown="0">
+  <autoFilter ref="A2:D8" xr:uid="{9B2A27B1-2ED2-454F-94FA-485094C1D042}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2D24D44B-B56F-43FE-AE79-607421C3669B}" name="id"/>
+    <tableColumn id="2" xr3:uid="{DAA76FAA-EE97-4582-8DA2-9ED09506F7AC}" name="name"/>
+    <tableColumn id="3" xr3:uid="{298EAFE0-C9F7-4809-A95C-4CF59365695C}" name="created_at"/>
+    <tableColumn id="4" xr3:uid="{0340B0B6-4A96-4DF1-9D95-AEC745409276}" name="modified_at"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{275A6343-742E-4AE1-9C15-4A4A14D2A6D9}" name="Tabla28" displayName="Tabla28" ref="A11:D44" totalsRowShown="0">
+  <autoFilter ref="A11:D44" xr:uid="{275A6343-742E-4AE1-9C15-4A4A14D2A6D9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BB4602CB-FC3C-4BDC-8AAE-C32E739A5154}" name="id"/>
+    <tableColumn id="2" xr3:uid="{8AEE5A29-B968-4494-9FCC-0E6D58C66643}" name="name"/>
+    <tableColumn id="3" xr3:uid="{F8743E7D-9162-462A-81B9-D77A9752A0E6}" name="created_at"/>
+    <tableColumn id="4" xr3:uid="{DDB41CC8-813A-4A5F-B867-77E4D6C5D443}" name="modified_at"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C78C286-6CA5-4893-B9A0-85015D3EB42D}" name="Tabla1" displayName="Tabla1" ref="A2:D8" totalsRowShown="0">
   <autoFilter ref="A2:D8" xr:uid="{0C78C286-6CA5-4893-B9A0-85015D3EB42D}"/>
   <tableColumns count="4">
@@ -1071,7 +1098,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{32AE777E-CAD0-4C9B-947D-EBE9586A670B}" name="Tabla2" displayName="Tabla2" ref="A11:D44" totalsRowShown="0">
   <autoFilter ref="A11:D44" xr:uid="{32AE777E-CAD0-4C9B-947D-EBE9586A670B}"/>
   <tableColumns count="4">
@@ -1084,7 +1111,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{38C728E8-8A8B-480C-BE15-0662FBB07D3F}" name="Tabla3" displayName="Tabla3" ref="A47:O57" totalsRowShown="0">
   <autoFilter ref="A47:O57" xr:uid="{38C728E8-8A8B-480C-BE15-0662FBB07D3F}"/>
   <tableColumns count="15">
@@ -1108,43 +1135,43 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{88F5B37B-C690-4917-88FD-048417BE3C8F}" name="Tabla4" displayName="Tabla4" ref="A60:AA70" totalsRowShown="0" headerRowDxfId="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{88F5B37B-C690-4917-88FD-048417BE3C8F}" name="Tabla4" displayName="Tabla4" ref="A60:AA70" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A60:AA70" xr:uid="{88F5B37B-C690-4917-88FD-048417BE3C8F}"/>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{6F50D45D-90E0-47A0-A3E3-165E1F67205D}" name="id" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{D9123418-7E69-4C38-A4BF-7938EFD19DFA}" name="tuid" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{322F73FE-A822-405A-B64B-734B60DFD1C7}" name="user_type_id" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{B121F4B0-4463-4051-BB04-2D2AC2C244AD}" name="user_parent_id" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{1F0A03EF-EEC4-4E78-A922-BEE67CFCEA8A}" name="user_relationship_id" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{9FE40679-7A4B-4704-BECF-9C42A61C63B3}" name="username" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{5A1E279B-348E-43B4-B617-6B207EB33473}" name="avatar" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{02736100-66B8-4ACB-B564-8FDC582DF303}" name="name" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{8742BCCA-FD95-442F-ADD6-A1FAAE69062E}" name="middlename" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{203DF922-87FB-4663-BB39-F2119AC097DC}" name="lastname" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{7773F394-78CF-4434-8167-D7949CCD6D63}" name="maidenname" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{5F6BF1AC-487E-4B97-92F7-6C055EACFDBB}" name="birthday" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{77959896-6D5D-4D24-BAFA-5E355BB21AF6}" name="emails" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{61A543C0-070F-4DC6-9D49-B6A460FC8C07}" name="phones" dataDxfId="14"/>
-    <tableColumn id="15" xr3:uid="{D7E13A03-A972-4952-B6A5-EDA4AFBB6719}" name="address" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{5314A568-B011-4E95-A456-81C7AD465563}" name="gender" dataDxfId="12"/>
-    <tableColumn id="17" xr3:uid="{1B9BB123-8500-4467-9DB1-FF8F7B14598B}" name="rfc" dataDxfId="11"/>
-    <tableColumn id="18" xr3:uid="{DFF901FB-15A0-4938-94AE-735B2F8C5C05}" name="isactive" dataDxfId="10"/>
-    <tableColumn id="19" xr3:uid="{F0CAB542-4957-4EAD-881B-CAF3C852BEF2}" name="isvalid" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{DD1FE52D-DC0D-412E-B132-C093F280F246}" name="referral_code" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{9A1EC1F9-C71F-4E57-AF96-337275F3DCF7}" name="created_at" dataDxfId="7"/>
-    <tableColumn id="22" xr3:uid="{FB148F4F-0C07-4029-AF7D-B709EA4C4897}" name="modified_at" dataDxfId="6"/>
-    <tableColumn id="23" xr3:uid="{EE671489-84E8-408C-8061-02C5CFFFCC33}" name="org_team_id" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{A5543D63-CD1B-4B79-9743-4BF9C9661D61}" name="toid" dataDxfId="4"/>
-    <tableColumn id="25" xr3:uid="{9E435C6C-BB7F-4BA2-8219-5D37AF32CF1B}" name="employe_no" dataDxfId="3"/>
-    <tableColumn id="26" xr3:uid="{AE978C7D-1C79-4C0F-A118-1259AEE637F3}" name="org_id" dataDxfId="2"/>
-    <tableColumn id="27" xr3:uid="{73BA4080-CD3A-4951-BA7F-78EBFA6670AF}" name="curp" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6F50D45D-90E0-47A0-A3E3-165E1F67205D}" name="id" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{D9123418-7E69-4C38-A4BF-7938EFD19DFA}" name="tuid" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{322F73FE-A822-405A-B64B-734B60DFD1C7}" name="user_type_id" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{B121F4B0-4463-4051-BB04-2D2AC2C244AD}" name="user_parent_id" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{1F0A03EF-EEC4-4E78-A922-BEE67CFCEA8A}" name="user_relationship_id" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{9FE40679-7A4B-4704-BECF-9C42A61C63B3}" name="username" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{5A1E279B-348E-43B4-B617-6B207EB33473}" name="avatar" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{02736100-66B8-4ACB-B564-8FDC582DF303}" name="name" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{8742BCCA-FD95-442F-ADD6-A1FAAE69062E}" name="middlename" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{203DF922-87FB-4663-BB39-F2119AC097DC}" name="lastname" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{7773F394-78CF-4434-8167-D7949CCD6D63}" name="maidenname" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{5F6BF1AC-487E-4B97-92F7-6C055EACFDBB}" name="birthday" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{77959896-6D5D-4D24-BAFA-5E355BB21AF6}" name="emails" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{61A543C0-070F-4DC6-9D49-B6A460FC8C07}" name="phones" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{D7E13A03-A972-4952-B6A5-EDA4AFBB6719}" name="address" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{5314A568-B011-4E95-A456-81C7AD465563}" name="gender" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{1B9BB123-8500-4467-9DB1-FF8F7B14598B}" name="rfc" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{DFF901FB-15A0-4938-94AE-735B2F8C5C05}" name="isactive" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{F0CAB542-4957-4EAD-881B-CAF3C852BEF2}" name="isvalid" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{DD1FE52D-DC0D-412E-B132-C093F280F246}" name="referral_code" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{9A1EC1F9-C71F-4E57-AF96-337275F3DCF7}" name="created_at" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{FB148F4F-0C07-4029-AF7D-B709EA4C4897}" name="modified_at" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{EE671489-84E8-408C-8061-02C5CFFFCC33}" name="org_team_id" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{A5543D63-CD1B-4B79-9743-4BF9C9661D61}" name="toid" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{9E435C6C-BB7F-4BA2-8219-5D37AF32CF1B}" name="employe_no" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{AE978C7D-1C79-4C0F-A118-1259AEE637F3}" name="org_id" dataDxfId="1"/>
+    <tableColumn id="27" xr3:uid="{73BA4080-CD3A-4951-BA7F-78EBFA6670AF}" name="curp" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9BD6FDEE-2986-4D6F-8401-497CCEEEFB98}" name="Tabla5" displayName="Tabla5" ref="A73:W83" totalsRowShown="0">
   <autoFilter ref="A73:W83" xr:uid="{9BD6FDEE-2986-4D6F-8401-497CCEEEFB98}"/>
   <tableColumns count="23">
@@ -1472,11 +1499,629 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D7E362-35FC-4D60-BFC7-8C1DF5B5CB35}">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>23</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>28</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>31</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>33</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FEB89B-63CB-4B66-866B-E79EC8D2DDF8}">
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="A12:B44"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Logs Module & Winston
</commit_message>
<xml_diff>
--- a/arq/Tablas_Significado.xlsx
+++ b/arq/Tablas_Significado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FZGC\AER_PassiDocs_Natural\arq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA0F3EC-1F67-48B8-943F-5DE37054B42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA9AFB3-AA10-401A-8C17-E75C5EFC80CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{690E9754-8DAB-491D-B572-8F25C1E44882}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="328">
   <si>
     <t>docs_group</t>
   </si>
@@ -904,13 +904,130 @@
   </si>
   <si>
     <t>users</t>
+  </si>
+  <si>
+    <t>segutiendasekurauploadfile</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>id_product</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>abbr_folder</t>
+  </si>
+  <si>
+    <t>AER</t>
+  </si>
+  <si>
+    <t>C:/FZGC/Pólizas_Ejemplo/(Auto-Primero)23110770685f3c-7bd4-4d47-b752-96e6bb7e6273.pdf</t>
+  </si>
+  <si>
+    <t>POST (form-data)</t>
+  </si>
+  <si>
+    <t>OPCIONAL</t>
+  </si>
+  <si>
+    <t>http://13.52.238.16:3000/segutiendasekurauploadfile</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "status": 200,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "isRaw": true,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "body": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "req": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "id_user": "3",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "id_product": "12345",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "docs_group": "6",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "timestamp": "2024-01-23 12:19:48.878+00",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "abbr_folder": "AER",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "url": "AER/users/3_12345_25_6_20231019.pdf",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "url_bucket": "https://resio.s3.amazonaws.com/AER/users/3_12345_25_6_20231019.pdf",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "ocrdoc_classify": "1_25_Flotillas_Primero",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "message": "Uploaded the file successfully: C:\\FZGC\\AER_PassiDocs_Natural\\resources\\static\\assets\\uploads\\(Auto-Primero)23110770685f3c-7bd4-4d47-b752-96e6bb7e6273.pdf"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "headers": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "Content-Type": "application/json"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>RESPUESTA SERVICIO</t>
+  </si>
+  <si>
+    <t>CATALOGO ERRORES</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>código</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Base de Datos No registro</t>
+  </si>
+  <si>
+    <t>Falta campo / recurso</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -918,8 +1035,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -932,8 +1065,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -941,21 +1092,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
@@ -1500,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D7E362-35FC-4D60-BFC7-8C1DF5B5CB35}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,17 +1682,25 @@
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1534,8 +1713,15 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1548,8 +1734,15 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1562,8 +1755,15 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1576,8 +1776,15 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="H5" s="2">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1590,8 +1797,17 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1604,8 +1820,15 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1618,16 +1841,34 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="H8" s="2">
+        <v>20231019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1640,8 +1881,12 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1654,8 +1899,12 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1668,8 +1917,12 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1682,8 +1935,12 @@
       <c r="D14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1696,8 +1953,12 @@
       <c r="D15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1710,8 +1971,12 @@
       <c r="D16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1724,8 +1989,12 @@
       <c r="D17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1738,8 +2007,12 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1752,8 +2025,12 @@
       <c r="D19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -1766,8 +2043,12 @@
       <c r="D20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1780,8 +2061,12 @@
       <c r="D21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1794,8 +2079,12 @@
       <c r="D22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="9"/>
+      <c r="G22" s="9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12</v>
       </c>
@@ -1808,8 +2097,12 @@
       <c r="D23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
@@ -1822,8 +2115,12 @@
       <c r="D24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" s="9"/>
+      <c r="G24" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>14</v>
       </c>
@@ -1836,8 +2133,12 @@
       <c r="D25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="9"/>
+      <c r="G25" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>15</v>
       </c>
@@ -1850,8 +2151,12 @@
       <c r="D26" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" s="9"/>
+      <c r="G26" s="9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>16</v>
       </c>
@@ -1864,8 +2169,12 @@
       <c r="D27" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" s="9"/>
+      <c r="G27" s="9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>17</v>
       </c>
@@ -1878,8 +2187,12 @@
       <c r="D28" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28" s="9"/>
+      <c r="G28" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>18</v>
       </c>
@@ -1892,8 +2205,12 @@
       <c r="D29" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F29" s="9"/>
+      <c r="G29" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>19</v>
       </c>
@@ -1906,8 +2223,12 @@
       <c r="D30" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" s="9"/>
+      <c r="G30" s="9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20</v>
       </c>
@@ -1920,8 +2241,12 @@
       <c r="D31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>21</v>
       </c>
@@ -1935,7 +2260,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>22</v>
       </c>
@@ -1949,7 +2274,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>23</v>
       </c>
@@ -1962,8 +2287,12 @@
       <c r="D34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>24</v>
       </c>
@@ -1976,8 +2305,14 @@
       <c r="D35" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>25</v>
       </c>
@@ -1990,8 +2325,14 @@
       <c r="D36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" s="9">
+        <v>200</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>26</v>
       </c>
@@ -2004,8 +2345,14 @@
       <c r="D37" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F37" s="9">
+        <v>204</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>27</v>
       </c>
@@ -2018,8 +2365,14 @@
       <c r="D38" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F38" s="9">
+        <v>400</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>28</v>
       </c>
@@ -2032,8 +2385,14 @@
       <c r="D39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F39" s="9">
+        <v>500</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>29</v>
       </c>
@@ -2047,7 +2406,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>30</v>
       </c>
@@ -2061,7 +2420,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>31</v>
       </c>
@@ -2075,7 +2434,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>32</v>
       </c>
@@ -2089,7 +2448,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>33</v>
       </c>
@@ -2104,14 +2463,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F34:G34"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{DE3B8169-1AB8-484A-9B71-E34B8957D292}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2146,12 +2510,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2252,12 +2616,12 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2736,23 +3100,23 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3173,35 +3537,35 @@
       </c>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
-      <c r="S59" s="2"/>
-      <c r="T59" s="2"/>
-      <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
-      <c r="W59" s="2"/>
-      <c r="X59" s="2"/>
-      <c r="Y59" s="2"/>
-      <c r="Z59" s="2"/>
-      <c r="AA59" s="2"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="5"/>
+      <c r="Z59" s="5"/>
+      <c r="AA59" s="5"/>
     </row>
     <row r="60" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -3779,31 +4143,31 @@
     </row>
     <row r="71" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="3"/>
-      <c r="O72" s="3"/>
-      <c r="P72" s="3"/>
-      <c r="Q72" s="3"/>
-      <c r="R72" s="3"/>
-      <c r="S72" s="3"/>
-      <c r="T72" s="3"/>
-      <c r="U72" s="3"/>
-      <c r="V72" s="3"/>
-      <c r="W72" s="3"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="7"/>
+      <c r="R72" s="7"/>
+      <c r="S72" s="7"/>
+      <c r="T72" s="7"/>
+      <c r="U72" s="7"/>
+      <c r="V72" s="7"/>
+      <c r="W72" s="7"/>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" t="s">

</xml_diff>